<commit_message>
acertando o registro da erva de s joao
</commit_message>
<xml_diff>
--- a/bianca-so-floracao-2025.xlsx
+++ b/bianca-so-floracao-2025.xlsx
@@ -249,7 +249,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -264,6 +264,9 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -698,8 +701,8 @@
       <c r="B7" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="3">
-        <v>0.0</v>
+      <c r="C7" s="5">
+        <v>1.0</v>
       </c>
       <c r="D7" s="2">
         <v>0.0</v>

</xml_diff>